<commit_message>
Fix league gold receiving bug
</commit_message>
<xml_diff>
--- a/const/monsters.xlsx
+++ b/const/monsters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="580" windowWidth="25600" windowHeight="16060" activeTab="1"/>
+    <workbookView xWindow="11860" yWindow="600" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="野怪组合列表" sheetId="1" r:id="rId1"/>
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -777,7 +777,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -800,7 +800,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -823,7 +823,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -846,7 +846,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D9" s="1">
         <v>2</v>
@@ -869,7 +869,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1">
         <v>2</v>
@@ -892,7 +892,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D11" s="1">
         <v>2</v>
@@ -915,7 +915,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1">
         <v>2</v>
@@ -937,8 +937,8 @@
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="1">
-        <v>4</v>
+      <c r="C13" s="3">
+        <v>5</v>
       </c>
       <c r="D13" s="1">
         <v>2</v>
@@ -960,7 +960,7 @@
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="3">
         <v>5</v>
       </c>
       <c r="D14" s="1">
@@ -983,7 +983,7 @@
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="3">
         <v>5</v>
       </c>
       <c r="D15" s="1">
@@ -1006,7 +1006,7 @@
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="3">
         <v>5</v>
       </c>
       <c r="D16" s="1">
@@ -1029,7 +1029,7 @@
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="3">
         <v>5</v>
       </c>
       <c r="D17" s="1">
@@ -1052,7 +1052,7 @@
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="3">
         <v>5</v>
       </c>
       <c r="D18" s="1">
@@ -1075,7 +1075,7 @@
       <c r="B19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="3">
         <v>5</v>
       </c>
       <c r="D19" s="1">
@@ -1202,7 +1202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>

</xml_diff>